<commit_message>
Create Survey updated by team 3
</commit_message>
<xml_diff>
--- a/Documentation/For database testing.xlsx
+++ b/Documentation/For database testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>size_min</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -280,6 +280,105 @@
   </si>
   <si>
     <t>photo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Satisfactory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>If the vaule is blank, please set  satisfactory_vUnsatisfactory=Very Unsatisfactory, satisfactory_Unsatisfactory=Unsatisfactory, satisfactory_Neutral=Neutral, satisfactory_Satisfactory=Satisfactory, satisfactory_vSatisfactory=Very Satisfactory</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">*** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>If the vaule is blank, please set as "NULL"</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>***</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> If the vaule is not blank, that means got URL, then save the value into database.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image Radio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type: "img_radio"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type: "satisfactory"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type:"img_checkbox"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image Checkbox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>satisfactory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>img_radio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>img_checkbox</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -718,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M57"/>
+  <dimension ref="A2:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -962,97 +1061,88 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C23" s="10" t="s">
-        <v>29</v>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C34" s="10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="C37" s="3"/>
+      <c r="A37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
@@ -1060,10 +1150,10 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1072,10 +1162,10 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1084,10 +1174,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,82 +1186,173 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="4"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="C54" s="3"/>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="C56" s="3"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>